<commit_message>
full generification of the three-level-stratification input table
</commit_message>
<xml_diff>
--- a/INPUT-FILES/SHIPLEY/adult-rawToSS.xlsx
+++ b/INPUT-FILES/SHIPLEY/adult-rawToSS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eklaassen\Desktop\Misc\Shipley norms task\For Dave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A78091-B398-42CF-AE07-9766DF7DB378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80596614-4A2D-4851-8E9B-35FE3847A3A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="204" sheetId="1" r:id="rId1"/>
@@ -14453,8 +14453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBDD183-BC91-40BC-BE71-284E8A951EEA}">
   <dimension ref="A1:F247"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15449,7 +15449,7 @@
         <v>112</v>
       </c>
       <c r="E84" s="2">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="F84" s="2">
         <v>45</v>
@@ -20206,7 +20206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CAE845-673F-42DD-9ED8-0E493A13D10F}">
   <dimension ref="A1:F256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>

</xml_diff>